<commit_message>
fix to pop file
</commit_message>
<xml_diff>
--- a/Data/Global Data/Population_Country2.xlsx
+++ b/Data/Global Data/Population_Country2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="266">
   <si>
     <t>'Zimbabwe'</t>
   </si>
@@ -527,9 +527,6 @@
     <t>'Afghanistan'</t>
   </si>
   <si>
-    <t>ï..Country</t>
-  </si>
-  <si>
     <t>matrixID</t>
   </si>
   <si>
@@ -819,6 +816,12 @@
   </si>
   <si>
     <t>'Paracel Islands'</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>x1990</t>
   </si>
 </sst>
 </file>
@@ -1138,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,13 +1152,13 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" t="s">
         <v>167</v>
       </c>
-      <c r="B1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1">
-        <v>1990</v>
+      <c r="C1" t="s">
+        <v>265</v>
       </c>
       <c r="D1">
         <v>1991</v>
@@ -1241,7 +1244,7 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1609,7 +1612,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1701,7 +1704,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1885,7 +1888,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1977,7 +1980,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -2253,7 +2256,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2345,7 +2348,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2897,7 +2900,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -2989,7 +2992,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -3633,7 +3636,7 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -3909,7 +3912,7 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -4185,7 +4188,7 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -4369,7 +4372,7 @@
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -4461,7 +4464,7 @@
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -5289,7 +5292,7 @@
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -5749,7 +5752,7 @@
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B51">
         <v>50</v>
@@ -5841,7 +5844,7 @@
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B52">
         <v>51</v>
@@ -5933,7 +5936,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B53">
         <v>52</v>
@@ -6393,7 +6396,7 @@
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B58">
         <v>57</v>
@@ -6485,7 +6488,7 @@
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B59">
         <v>58</v>
@@ -6761,7 +6764,7 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B62">
         <v>61</v>
@@ -6853,7 +6856,7 @@
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B63">
         <v>62</v>
@@ -7129,7 +7132,7 @@
     </row>
     <row r="66" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B66">
         <v>65</v>
@@ -7405,7 +7408,7 @@
     </row>
     <row r="69" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B69">
         <v>68</v>
@@ -8233,7 +8236,7 @@
     </row>
     <row r="78" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B78">
         <v>77</v>
@@ -8325,7 +8328,7 @@
     </row>
     <row r="79" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B79">
         <v>78</v>
@@ -8417,7 +8420,7 @@
     </row>
     <row r="80" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B80">
         <v>79</v>
@@ -8509,7 +8512,7 @@
     </row>
     <row r="81" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B81">
         <v>80</v>
@@ -8877,7 +8880,7 @@
     </row>
     <row r="85" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B85">
         <v>84</v>
@@ -8969,7 +8972,7 @@
     </row>
     <row r="86" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B86">
         <v>85</v>
@@ -9061,7 +9064,7 @@
     </row>
     <row r="87" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B87">
         <v>86</v>
@@ -9337,7 +9340,7 @@
     </row>
     <row r="90" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B90">
         <v>89</v>
@@ -9705,7 +9708,7 @@
     </row>
     <row r="94" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B94">
         <v>93</v>
@@ -9797,7 +9800,7 @@
     </row>
     <row r="95" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B95">
         <v>94</v>
@@ -9981,7 +9984,7 @@
     </row>
     <row r="97" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B97">
         <v>96</v>
@@ -10073,7 +10076,7 @@
     </row>
     <row r="98" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B98">
         <v>97</v>
@@ -10165,7 +10168,7 @@
     </row>
     <row r="99" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B99">
         <v>98</v>
@@ -10257,7 +10260,7 @@
     </row>
     <row r="100" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B100">
         <v>99</v>
@@ -10441,7 +10444,7 @@
     </row>
     <row r="102" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B102">
         <v>101</v>
@@ -10901,7 +10904,7 @@
     </row>
     <row r="107" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B107">
         <v>106</v>
@@ -11085,7 +11088,7 @@
     </row>
     <row r="109" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B109">
         <v>108</v>
@@ -11177,7 +11180,7 @@
     </row>
     <row r="110" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B110">
         <v>109</v>
@@ -11913,7 +11916,7 @@
     </row>
     <row r="118" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B118">
         <v>117</v>
@@ -12373,7 +12376,7 @@
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B123">
         <v>122</v>
@@ -12465,7 +12468,7 @@
     </row>
     <row r="124" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B124">
         <v>123</v>
@@ -12557,7 +12560,7 @@
     </row>
     <row r="125" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B125">
         <v>124</v>
@@ -12741,7 +12744,7 @@
     </row>
     <row r="127" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B127">
         <v>126</v>
@@ -13017,7 +13020,7 @@
     </row>
     <row r="130" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B130">
         <v>129</v>
@@ -13109,7 +13112,7 @@
     </row>
     <row r="131" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B131">
         <v>130</v>
@@ -13937,7 +13940,7 @@
     </row>
     <row r="140" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B140">
         <v>139</v>
@@ -14213,7 +14216,7 @@
     </row>
     <row r="143" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B143">
         <v>142</v>
@@ -14949,7 +14952,7 @@
     </row>
     <row r="151" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B151">
         <v>150</v>
@@ -15041,7 +15044,7 @@
     </row>
     <row r="152" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B152">
         <v>151</v>
@@ -15317,7 +15320,7 @@
     </row>
     <row r="155" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B155">
         <v>154</v>
@@ -15501,7 +15504,7 @@
     </row>
     <row r="157" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B157">
         <v>156</v>
@@ -15685,7 +15688,7 @@
     </row>
     <row r="159" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B159">
         <v>158</v>
@@ -15961,7 +15964,7 @@
     </row>
     <row r="162" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B162">
         <v>161</v>
@@ -16329,7 +16332,7 @@
     </row>
     <row r="166" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B166">
         <v>165</v>
@@ -16421,7 +16424,7 @@
     </row>
     <row r="167" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B167">
         <v>166</v>
@@ -16697,7 +16700,7 @@
     </row>
     <row r="170" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B170">
         <v>169</v>
@@ -17157,7 +17160,7 @@
     </row>
     <row r="175" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B175">
         <v>174</v>
@@ -17249,7 +17252,7 @@
     </row>
     <row r="176" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B176">
         <v>175</v>
@@ -17341,7 +17344,7 @@
     </row>
     <row r="177" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B177">
         <v>176</v>
@@ -17433,7 +17436,7 @@
     </row>
     <row r="178" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B178">
         <v>177</v>
@@ -17801,7 +17804,7 @@
     </row>
     <row r="182" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B182">
         <v>181</v>
@@ -17893,7 +17896,7 @@
     </row>
     <row r="183" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B183">
         <v>182</v>
@@ -17985,7 +17988,7 @@
     </row>
     <row r="184" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B184">
         <v>183</v>
@@ -18537,7 +18540,7 @@
     </row>
     <row r="190" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B190">
         <v>189</v>
@@ -18813,7 +18816,7 @@
     </row>
     <row r="193" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B193">
         <v>192</v>
@@ -18997,7 +19000,7 @@
     </row>
     <row r="195" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B195">
         <v>194</v>
@@ -19365,7 +19368,7 @@
     </row>
     <row r="199" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B199">
         <v>198</v>
@@ -19457,7 +19460,7 @@
     </row>
     <row r="200" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B200">
         <v>199</v>
@@ -19549,7 +19552,7 @@
     </row>
     <row r="201" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B201">
         <v>200</v>
@@ -19733,7 +19736,7 @@
     </row>
     <row r="203" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B203">
         <v>202</v>
@@ -19825,7 +19828,7 @@
     </row>
     <row r="204" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B204">
         <v>203</v>
@@ -20101,7 +20104,7 @@
     </row>
     <row r="207" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B207">
         <v>206</v>
@@ -20469,7 +20472,7 @@
     </row>
     <row r="211" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B211">
         <v>210</v>
@@ -20561,7 +20564,7 @@
     </row>
     <row r="212" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B212">
         <v>211</v>
@@ -20837,7 +20840,7 @@
     </row>
     <row r="215" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B215">
         <v>214</v>
@@ -20929,7 +20932,7 @@
     </row>
     <row r="216" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B216">
         <v>215</v>
@@ -21205,7 +21208,7 @@
     </row>
     <row r="219" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B219">
         <v>218</v>
@@ -21389,7 +21392,7 @@
     </row>
     <row r="221" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B221">
         <v>220</v>
@@ -21665,7 +21668,7 @@
     </row>
     <row r="224" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B224">
         <v>223</v>
@@ -21849,7 +21852,7 @@
     </row>
     <row r="226" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B226">
         <v>225</v>
@@ -22033,7 +22036,7 @@
     </row>
     <row r="228" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B228">
         <v>227</v>
@@ -22401,7 +22404,7 @@
     </row>
     <row r="232" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B232">
         <v>231</v>
@@ -22493,7 +22496,7 @@
     </row>
     <row r="233" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B233">
         <v>232</v>
@@ -23045,7 +23048,7 @@
     </row>
     <row r="239" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B239">
         <v>238</v>
@@ -23321,7 +23324,7 @@
     </row>
     <row r="242" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B242">
         <v>241</v>
@@ -23689,7 +23692,7 @@
     </row>
     <row r="246" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B246">
         <v>245</v>
@@ -23781,7 +23784,7 @@
     </row>
     <row r="247" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B247">
         <v>246</v>
@@ -24517,7 +24520,7 @@
     </row>
     <row r="255" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B255">
         <v>254</v>
@@ -24793,7 +24796,7 @@
     </row>
     <row r="258" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B258">
         <v>257</v>
@@ -24885,7 +24888,7 @@
     </row>
     <row r="259" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B259">
         <v>258</v>
@@ -24977,7 +24980,7 @@
     </row>
     <row r="260" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B260">
         <v>259</v>
@@ -25069,7 +25072,7 @@
     </row>
     <row r="261" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B261">
         <v>260</v>
@@ -25437,7 +25440,7 @@
     </row>
     <row r="265" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B265">
         <v>264</v>

</xml_diff>